<commit_message>
update DB theo y kien VietBQ
</commit_message>
<xml_diff>
--- a/Prj_ERROR404/02_Member/LuanNT/20140911_DatabaseDesign/CSDL.xlsx
+++ b/Prj_ERROR404/02_Member/LuanNT/20140911_DatabaseDesign/CSDL.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
   <si>
     <t>Tác giả</t>
   </si>
@@ -138,48 +138,21 @@
     <t>Thuộc tính</t>
   </si>
   <si>
-    <t>ID_Author</t>
-  </si>
-  <si>
     <t>author</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>IMG</t>
-  </si>
-  <si>
     <t>biography</t>
   </si>
   <si>
     <t>ID_Book</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Remain</t>
-  </si>
-  <si>
-    <t>Adult</t>
-  </si>
-  <si>
-    <t>Ebook</t>
-  </si>
-  <si>
     <t>eBook</t>
   </si>
   <si>
     <t>authorWroteBook</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>MailAddress</t>
-  </si>
-  <si>
     <t>UserBoughtBook</t>
   </si>
   <si>
@@ -237,7 +210,64 @@
     <t>true Nam,False Nữ</t>
   </si>
   <si>
-    <t>varchar</t>
+    <t>id_author</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>id_book</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>adult</t>
+  </si>
+  <si>
+    <t>ebook</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>dateofbirth</t>
+  </si>
+  <si>
+    <t>mailaddress</t>
+  </si>
+  <si>
+    <t>id_user</t>
+  </si>
+  <si>
+    <t>acccreateddate</t>
+  </si>
+  <si>
+    <t>nearestsignin</t>
+  </si>
+  <si>
+    <t>balance</t>
+  </si>
+  <si>
+    <t>id_category</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>descriptionofprofessional</t>
+  </si>
+  <si>
+    <t>descriptionof404</t>
   </si>
 </sst>
 </file>
@@ -327,8 +357,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E52" totalsRowShown="0">
-  <autoFilter ref="A1:E52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E55" totalsRowShown="0">
+  <autoFilter ref="A1:E55">
     <filterColumn colId="1"/>
     <filterColumn colId="3"/>
   </autoFilter>
@@ -628,16 +658,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="66.42578125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
@@ -651,10 +681,10 @@
         <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
         <v>31</v>
@@ -665,39 +695,39 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="B4" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -705,13 +735,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="B5" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -727,13 +757,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -741,46 +771,46 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="B11" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="B12" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
         <v>32</v>
@@ -788,13 +818,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="B13" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -802,13 +832,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="B14" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>7</v>
@@ -816,359 +846,386 @@
     </row>
     <row r="15" spans="1:5">
       <c r="B15" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="16" spans="1:5">
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
     <row r="17" spans="1:5">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="D20" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>28</v>
+        <v>44</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" t="s">
-        <v>68</v>
-      </c>
+      <c r="A22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>69</v>
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>70</v>
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>59</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1"/>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D31" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="D34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="C33" s="3" t="s">
+    <row r="36" spans="1:5">
+      <c r="C36" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" t="s">
+      <c r="D36" s="3"/>
+      <c r="E36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" t="s">
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B40" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="4" t="s">
+      <c r="D40" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="B41" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E39" t="s">
-        <v>35</v>
+      <c r="D41" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B45" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="8" t="s">
+      <c r="D45" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
+      <c r="D46" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48" t="s">
-        <v>42</v>
-      </c>
-      <c r="C48" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>45</v>
+        <v>79</v>
+      </c>
+      <c r="C50" t="s">
+        <v>10</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>64</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
đổi tên thuộc tính CSDL.xlsx
</commit_message>
<xml_diff>
--- a/Prj_ERROR404/02_Member/LuanNT/20140911_DatabaseDesign/CSDL.xlsx
+++ b/Prj_ERROR404/02_Member/LuanNT/20140911_DatabaseDesign/CSDL.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="91">
   <si>
     <t>Tác giả</t>
   </si>
@@ -268,13 +268,34 @@
   </si>
   <si>
     <t>description404</t>
+  </si>
+  <si>
+    <t>VietBQ</t>
+  </si>
+  <si>
+    <t>vip</t>
+  </si>
+  <si>
+    <t>% giảm giá</t>
+  </si>
+  <si>
+    <t>nearest</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>birth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +330,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF3E454C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -336,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -347,6 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,14 +385,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E55" totalsRowShown="0">
-  <autoFilter ref="A1:E55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F55" totalsRowShown="0">
+  <autoFilter ref="A1:F55">
     <filterColumn colId="1"/>
-    <filterColumn colId="3"/>
+    <filterColumn colId="2"/>
+    <filterColumn colId="4"/>
   </autoFilter>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" name="Bảng"/>
     <tableColumn id="4" name="Thuộc tính"/>
+    <tableColumn id="5" name="VietBQ"/>
     <tableColumn id="2" name="thuộc tính (tiếng việt)"/>
     <tableColumn id="6" name="Type"/>
     <tableColumn id="3" name="Mô tả"/>
@@ -658,22 +688,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="66.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -681,78 +711,93 @@
         <v>39</v>
       </c>
       <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>65</v>
       </c>
       <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>59</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="B5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="C6" s="2"/>
+    <row r="6" spans="1:6">
       <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="C7" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -760,13 +805,16 @@
         <v>66</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -774,132 +822,165 @@
         <v>53</v>
       </c>
       <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="B10" t="s">
         <v>65</v>
       </c>
       <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
         <v>2</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="B11" t="s">
         <v>67</v>
       </c>
       <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="B13" t="s">
         <v>68</v>
       </c>
       <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>61</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="B14" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="B15" t="s">
         <v>70</v>
       </c>
       <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" t="s">
         <v>27</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
         <v>81</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6">
       <c r="B17" t="s">
         <v>82</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6">
       <c r="B18" t="s">
         <v>83</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -907,13 +988,16 @@
         <v>66</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
@@ -921,15 +1005,17 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -937,68 +1023,83 @@
         <v>75</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>17</v>
@@ -1007,61 +1108,74 @@
         <v>17</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:6">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>22</v>
@@ -1069,23 +1183,37 @@
       <c r="C34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
-      <c r="C36" s="3" t="s">
+    <row r="35" spans="1:6">
+      <c r="C35" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="D36" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" t="s">
+      <c r="E36" s="3"/>
+      <c r="F36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -1093,13 +1221,16 @@
         <v>75</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1107,13 +1238,16 @@
         <v>66</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="E41" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -1121,16 +1255,19 @@
         <v>67</v>
       </c>
       <c r="C42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" t="s">
         <v>34</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -1138,13 +1275,16 @@
         <v>75</v>
       </c>
       <c r="C45" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:6">
       <c r="A46" s="7" t="s">
         <v>46</v>
       </c>
@@ -1152,33 +1292,39 @@
         <v>66</v>
       </c>
       <c r="C46" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="E46" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1189,10 +1335,13 @@
         <v>53</v>
       </c>
       <c r="D51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E51" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -1200,13 +1349,16 @@
         <v>66</v>
       </c>
       <c r="C53" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="E53" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1214,18 +1366,22 @@
         <v>79</v>
       </c>
       <c r="C54" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="E54" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:6">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>